<commit_message>
Basic template of table
</commit_message>
<xml_diff>
--- a/5steps/fincalc.xlsx
+++ b/5steps/fincalc.xlsx
@@ -25,8 +25,67 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Калькулятор расчета ежемесячной прибыли по деозиту</t>
+  </si>
+  <si>
+    <t>Процентная ставка, %</t>
+  </si>
+  <si>
+    <t>Сумма депозита, грн</t>
+  </si>
+  <si>
+    <t>Месяц</t>
+  </si>
+  <si>
+    <t>Размер вклада, грн</t>
+  </si>
+  <si>
+    <t>январь</t>
+  </si>
+  <si>
+    <t>февраль</t>
+  </si>
+  <si>
+    <t>март</t>
+  </si>
+  <si>
+    <t>апрель</t>
+  </si>
+  <si>
+    <t>май</t>
+  </si>
+  <si>
+    <t>июнь</t>
+  </si>
+  <si>
+    <t>июль</t>
+  </si>
+  <si>
+    <t>август</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сентябрь</t>
+  </si>
+  <si>
+    <t>октябрь</t>
+  </si>
+  <si>
+    <t>ноябрь</t>
+  </si>
+  <si>
+    <t>декабрь</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$UAH]\ #,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -56,8 +115,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,13 +414,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="6">
+        <f>D3*D4%/12+D3</f>
+        <v>100916.66666666667</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <f>C7*D4%/12+C7</f>
+        <v>101841.73611111111</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>